<commit_message>
Tentative avec une banque un peu intelligente. Mais c'est pas top du tout, voie a oublier
</commit_message>
<xml_diff>
--- a/policy_compteur.xlsx
+++ b/policy_compteur.xlsx
@@ -555,8 +555,8 @@
       <c r="D4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>1</v>
+      <c r="E4" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>1</v>
@@ -573,8 +573,8 @@
       <c r="J4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="3" t="n">
-        <v>0</v>
+      <c r="K4" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>0</v>
@@ -602,23 +602,23 @@
       <c r="C5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>2</v>
+      <c r="D5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>0</v>
+      <c r="G5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J5" s="3" t="n">
         <v>0</v>
@@ -652,11 +652,11 @@
       <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>2</v>
+      <c r="D6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>1</v>
@@ -664,8 +664,8 @@
       <c r="G6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="3" t="n">
-        <v>0</v>
+      <c r="H6" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="I6" s="3" t="n">
         <v>0</v>
@@ -711,11 +711,11 @@
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>0</v>
+      <c r="G7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="I7" s="3" t="n">
         <v>0</v>
@@ -752,23 +752,23 @@
       <c r="C8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="n">
-        <v>0</v>
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J8" s="3" t="n">
         <v>0</v>
@@ -802,23 +802,23 @@
       <c r="C9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="n">
-        <v>2</v>
+      <c r="D9" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="n">
-        <v>0</v>
+      <c r="F9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J9" s="3" t="n">
         <v>0</v>
@@ -855,8 +855,8 @@
       <c r="D10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="4" t="n">
-        <v>2</v>
+      <c r="E10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1</v>
@@ -905,8 +905,8 @@
       <c r="D11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="4" t="n">
-        <v>2</v>
+      <c r="E11" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>1</v>
@@ -923,8 +923,8 @@
       <c r="J11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K11" s="2" t="n">
-        <v>1</v>
+      <c r="K11" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="L11" s="3" t="n">
         <v>0</v>
@@ -949,11 +949,11 @@
       <c r="B12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>2</v>
+      <c r="C12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>1</v>
@@ -996,17 +996,17 @@
       <c r="A13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="n">
-        <v>0</v>
+      <c r="B13" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4" t="n">
-        <v>2</v>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>1</v>
@@ -1102,8 +1102,8 @@
       <c r="F18" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G18" s="3" t="n">
-        <v>0</v>
+      <c r="G18" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H18" s="3" t="n">
         <v>0</v>
@@ -1183,8 +1183,8 @@
       <c r="A21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B21" s="4" t="n">
-        <v>2</v>
+      <c r="B21" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>1</v>
@@ -1218,20 +1218,20 @@
       <c r="B22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C22" s="4" t="n">
-        <v>2</v>
+      <c r="C22" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="4" t="n">
-        <v>2</v>
+      <c r="E22" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G22" s="4" t="n">
-        <v>2</v>
+      <c r="G22" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="H22" s="3" t="n">
         <v>0</v>
@@ -1262,8 +1262,8 @@
       <c r="F23" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G23" s="4" t="n">
-        <v>2</v>
+      <c r="G23" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="H23" s="3" t="n">
         <v>0</v>
@@ -1390,8 +1390,8 @@
       <c r="F27" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G27" s="2" t="n">
-        <v>1</v>
+      <c r="G27" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="H27" s="3" t="n">
         <v>0</v>
@@ -1451,8 +1451,8 @@
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="2" t="n">
-        <v>1</v>
+      <c r="B32" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>1</v>
@@ -1498,11 +1498,11 @@
       <c r="E33" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F33" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="3" t="n">
-        <v>0</v>
+      <c r="F33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="H33" s="5" t="n">
         <v>3</v>
@@ -1533,8 +1533,8 @@
       <c r="E34" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="4" t="n">
-        <v>2</v>
+      <c r="F34" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>1</v>
@@ -1556,11 +1556,11 @@
       <c r="A35" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B35" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C35" s="2" t="n">
-        <v>1</v>
+      <c r="B35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>1</v>
@@ -1568,14 +1568,14 @@
       <c r="E35" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F35" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3" t="n">
-        <v>0</v>
+      <c r="F35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H35" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="I35" s="5" t="n">
         <v>3</v>
@@ -1591,14 +1591,14 @@
       <c r="A36" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B36" s="2" t="n">
-        <v>1</v>
+      <c r="B36" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D36" s="2" t="n">
-        <v>1</v>
+      <c r="D36" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>1</v>
@@ -1606,8 +1606,8 @@
       <c r="F36" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="2" t="n">
-        <v>1</v>
+      <c r="G36" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="H36" s="5" t="n">
         <v>3</v>
@@ -1626,23 +1626,23 @@
       <c r="A37" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B37" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C37" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>1</v>
+      <c r="B37" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F37" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G37" s="5" t="n">
-        <v>3</v>
+      <c r="F37" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H37" s="5" t="n">
         <v>3</v>
@@ -1650,8 +1650,8 @@
       <c r="I37" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="J37" s="5" t="n">
-        <v>3</v>
+      <c r="J37" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="K37" s="3" t="n">
         <v>0</v>
@@ -1673,8 +1673,8 @@
       <c r="E38" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F38" s="4" t="n">
-        <v>2</v>
+      <c r="F38" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>1</v>
@@ -1702,14 +1702,14 @@
       <c r="C39" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D39" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" s="4" t="n">
-        <v>2</v>
+      <c r="D39" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>1</v>
@@ -1752,11 +1752,11 @@
       <c r="H40" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I40" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="5" t="n">
-        <v>3</v>
+      <c r="I40" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="K40" s="3" t="n">
         <v>0</v>
@@ -1778,8 +1778,8 @@
       <c r="E41" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F41" s="2" t="n">
-        <v>1</v>
+      <c r="F41" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>1</v>
@@ -1787,8 +1787,8 @@
       <c r="H41" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I41" s="3" t="n">
-        <v>0</v>
+      <c r="I41" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="J41" s="3" t="n">
         <v>0</v>

</xml_diff>